<commit_message>
docs : final docs
</commit_message>
<xml_diff>
--- a/Docs/Requirement List.xlsx
+++ b/Docs/Requirement List.xlsx
@@ -30,7 +30,7 @@
     <t>김수현</t>
   </si>
   <si>
-    <t>자전거 대여 정보 조회 기능, 자전거 예약대기 정보 조회/취소 기능, 자전거 반납 및 식당 예약 서비스 연계 기능, 결제 기능의 requirement list, use case diagrams,  use case descriptions</t>
+    <t>자전거 대여 정보 조회 기능, 자전거 예약대기 정보 조회/취소 기능, 자전거 반납 및 식당 예약 서비스 연계 기능, 결제 기능의 requirement list, use case diagrams,  use case descriptions, github history 파일 출력</t>
   </si>
   <si>
     <t>박지원</t>
@@ -1368,16 +1368,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:A29 B2:C25">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>